<commit_message>
Fixing problems with commands
</commit_message>
<xml_diff>
--- a/Documents/ControlUnit commands.xlsx
+++ b/Documents/ControlUnit commands.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="106">
   <si>
     <t>00000000</t>
   </si>
@@ -330,6 +330,9 @@
   </si>
   <si>
     <t>011 - (Z/C/E/L/STACK_H) WRITE BUS</t>
+  </si>
+  <si>
+    <t>1 - WRITE TO ALU</t>
   </si>
 </sst>
 </file>
@@ -606,23 +609,23 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -921,7 +924,7 @@
   <dimension ref="A1:K106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+      <selection activeCell="C9" activeCellId="1" sqref="C6 C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -956,10 +959,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="35">
         <v>0</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -976,8 +979,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="18.75">
-      <c r="A3" s="32"/>
-      <c r="B3" s="33"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="11" t="s">
         <v>37</v>
       </c>
@@ -992,8 +995,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A4" s="32"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="14" t="s">
         <v>38</v>
       </c>
@@ -1008,10 +1011,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="18.75">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="35">
         <v>1</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -1028,10 +1031,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="18.75">
-      <c r="A6" s="32"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="11" t="s">
-        <v>37</v>
+        <v>105</v>
       </c>
       <c r="E6" s="23" t="s">
         <v>4</v>
@@ -1044,8 +1047,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A7" s="32"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="14" t="s">
         <v>38</v>
       </c>
@@ -1060,10 +1063,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="18.75">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="35">
         <v>2</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -1078,10 +1081,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="18.75">
-      <c r="A9" s="32"/>
-      <c r="B9" s="33"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="11" t="s">
-        <v>37</v>
+        <v>105</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>8</v>
@@ -1094,8 +1097,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A10" s="32"/>
-      <c r="B10" s="33"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="14" t="s">
         <v>38</v>
       </c>
@@ -1108,10 +1111,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="18.75">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B11" s="35">
         <v>3</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -1126,8 +1129,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="11" t="s">
         <v>37</v>
       </c>
@@ -1140,8 +1143,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="14" t="s">
         <v>38</v>
       </c>
@@ -1154,10 +1157,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="35">
         <v>4</v>
       </c>
       <c r="C14" s="15" t="s">
@@ -1172,8 +1175,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75">
-      <c r="A15" s="34"/>
-      <c r="B15" s="33"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="16" t="s">
         <v>37</v>
       </c>
@@ -1186,8 +1189,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A16" s="34"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="17" t="s">
         <v>38</v>
       </c>
@@ -1200,10 +1203,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="18.75">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="33">
+      <c r="B17" s="35">
         <v>5</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -1213,35 +1216,35 @@
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:7" ht="18.75">
-      <c r="A18" s="32"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="11" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
     </row>
     <row r="19" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A19" s="32"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="36" t="s">
+      <c r="E19" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
     </row>
     <row r="20" spans="1:7" ht="18.75">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="33">
+      <c r="B20" s="35">
         <v>6</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -1249,40 +1252,40 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="18.75">
-      <c r="A21" s="32"/>
-      <c r="B21" s="33"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="11" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A22" s="32"/>
-      <c r="B22" s="33"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="25" t="s">
         <v>38</v>
       </c>
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="32"/>
-      <c r="B23" s="33"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="26"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="32"/>
-      <c r="B24" s="33"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="27"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" thickBot="1">
-      <c r="A25" s="32"/>
-      <c r="B25" s="33"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="28"/>
     </row>
     <row r="26" spans="1:7" ht="18.75">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="32" t="s">
         <v>42</v>
       </c>
       <c r="C26" s="21" t="s">
@@ -1290,38 +1293,38 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="18.75">
-      <c r="A27" s="32"/>
-      <c r="B27" s="31"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="32"/>
       <c r="C27" s="11" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18.75">
-      <c r="A28" s="32"/>
-      <c r="B28" s="31"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="32"/>
       <c r="C28" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="18.75">
-      <c r="A29" s="32"/>
-      <c r="B29" s="31"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="32"/>
       <c r="C29" s="12" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A30" s="32"/>
-      <c r="B30" s="31"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="32"/>
       <c r="C30" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="18.75">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="32" t="s">
         <v>47</v>
       </c>
       <c r="C31" s="20" t="s">
@@ -1329,51 +1332,51 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="18.75">
-      <c r="A32" s="32"/>
-      <c r="B32" s="31"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="32"/>
       <c r="C32" s="12" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="18.75">
-      <c r="A33" s="32"/>
-      <c r="B33" s="31"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="32"/>
       <c r="C33" s="16" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="19.5" thickBot="1">
-      <c r="A34" s="32"/>
-      <c r="B34" s="31"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="32"/>
       <c r="C34" s="13" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="18.75">
-      <c r="A35" s="32"/>
-      <c r="B35" s="31"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="32"/>
       <c r="C35" s="10"/>
     </row>
     <row r="36" spans="1:3" ht="18.75">
-      <c r="A36" s="32"/>
-      <c r="B36" s="31"/>
+      <c r="A36" s="31"/>
+      <c r="B36" s="32"/>
       <c r="C36" s="11"/>
     </row>
     <row r="37" spans="1:3" ht="18.75">
-      <c r="A37" s="32"/>
-      <c r="B37" s="31"/>
+      <c r="A37" s="31"/>
+      <c r="B37" s="32"/>
       <c r="C37" s="12"/>
     </row>
     <row r="38" spans="1:3" ht="19.5" thickBot="1">
-      <c r="A38" s="32"/>
-      <c r="B38" s="31"/>
+      <c r="A38" s="31"/>
+      <c r="B38" s="32"/>
       <c r="C38" s="13"/>
     </row>
     <row r="39" spans="1:3" ht="18.75">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="32" t="s">
         <v>52</v>
       </c>
       <c r="C39" s="10" t="s">
@@ -1381,45 +1384,45 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="18.75">
-      <c r="A40" s="32"/>
-      <c r="B40" s="31"/>
+      <c r="A40" s="31"/>
+      <c r="B40" s="32"/>
       <c r="C40" s="11" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="18.75">
-      <c r="A41" s="32"/>
-      <c r="B41" s="31"/>
+      <c r="A41" s="31"/>
+      <c r="B41" s="32"/>
       <c r="C41" s="21" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="18.75">
-      <c r="A42" s="32"/>
-      <c r="B42" s="31"/>
+      <c r="A42" s="31"/>
+      <c r="B42" s="32"/>
       <c r="C42" s="11" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="18.75">
-      <c r="A43" s="32"/>
-      <c r="B43" s="31"/>
+      <c r="A43" s="31"/>
+      <c r="B43" s="32"/>
       <c r="C43" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="19.5" thickBot="1">
-      <c r="A44" s="32"/>
-      <c r="B44" s="31"/>
+      <c r="A44" s="31"/>
+      <c r="B44" s="32"/>
       <c r="C44" s="19" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="18.75">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="B45" s="31" t="s">
+      <c r="B45" s="32" t="s">
         <v>60</v>
       </c>
       <c r="C45" s="10" t="s">
@@ -1427,59 +1430,59 @@
       </c>
     </row>
     <row r="46" spans="1:3" ht="18.75">
-      <c r="A46" s="32"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="11" t="s">
+      <c r="A46" s="31"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="12" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="18.75">
-      <c r="A47" s="32"/>
-      <c r="B47" s="31"/>
+      <c r="A47" s="31"/>
+      <c r="B47" s="32"/>
       <c r="C47" s="11" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="18.75">
-      <c r="A48" s="32"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="11" t="s">
+      <c r="A48" s="31"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="12" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="18.75">
-      <c r="A49" s="32"/>
-      <c r="B49" s="31"/>
+      <c r="A49" s="31"/>
+      <c r="B49" s="32"/>
       <c r="C49" s="12" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="18.75">
-      <c r="A50" s="32"/>
-      <c r="B50" s="31"/>
+      <c r="A50" s="31"/>
+      <c r="B50" s="32"/>
       <c r="C50" s="12" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="18.75">
-      <c r="A51" s="32"/>
-      <c r="B51" s="31"/>
+      <c r="A51" s="31"/>
+      <c r="B51" s="32"/>
       <c r="C51" s="11" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="19.5" thickBot="1">
-      <c r="A52" s="32"/>
-      <c r="B52" s="31"/>
+      <c r="A52" s="31"/>
+      <c r="B52" s="32"/>
       <c r="C52" s="14" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="18.75">
-      <c r="A53" s="32" t="s">
+      <c r="A53" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="B53" s="31" t="s">
+      <c r="B53" s="32" t="s">
         <v>63</v>
       </c>
       <c r="C53" s="15" t="s">
@@ -1487,36 +1490,36 @@
       </c>
     </row>
     <row r="54" spans="1:3" ht="18.75">
-      <c r="A54" s="32"/>
-      <c r="B54" s="31"/>
+      <c r="A54" s="31"/>
+      <c r="B54" s="32"/>
       <c r="C54" s="11" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="18.75">
-      <c r="A55" s="32"/>
-      <c r="B55" s="31"/>
+      <c r="A55" s="31"/>
+      <c r="B55" s="32"/>
       <c r="C55" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="18.75">
-      <c r="A56" s="32"/>
-      <c r="B56" s="31"/>
+      <c r="A56" s="31"/>
+      <c r="B56" s="32"/>
       <c r="C56" s="11" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="18.75">
-      <c r="A57" s="32"/>
-      <c r="B57" s="31"/>
+      <c r="A57" s="31"/>
+      <c r="B57" s="32"/>
       <c r="C57" s="12" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="19.5" thickBot="1">
-      <c r="A58" s="32"/>
-      <c r="B58" s="31"/>
+      <c r="A58" s="31"/>
+      <c r="B58" s="32"/>
       <c r="C58" s="13" t="s">
         <v>68</v>
       </c>
@@ -1588,6 +1591,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A8:A10"/>
     <mergeCell ref="A53:A58"/>
     <mergeCell ref="B53:B58"/>
     <mergeCell ref="E18:G18"/>
@@ -1604,20 +1621,6 @@
     <mergeCell ref="B17:B19"/>
     <mergeCell ref="B45:B52"/>
     <mergeCell ref="A45:A52"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
@@ -1628,8 +1631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1663,10 +1666,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="33">
+      <c r="B2" s="35">
         <v>0</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -1683,8 +1686,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="18.75">
-      <c r="A3" s="32"/>
-      <c r="B3" s="33"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="35"/>
       <c r="C3" s="11" t="s">
         <v>37</v>
       </c>
@@ -1699,8 +1702,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A4" s="32"/>
-      <c r="B4" s="33"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="14" t="s">
         <v>38</v>
       </c>
@@ -1715,10 +1718,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="18.75">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="31" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="35">
         <v>1</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -1735,10 +1738,10 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="18.75">
-      <c r="A6" s="32"/>
-      <c r="B6" s="33"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="11" t="s">
-        <v>37</v>
+        <v>105</v>
       </c>
       <c r="E6" s="23" t="s">
         <v>4</v>
@@ -1751,8 +1754,8 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A7" s="32"/>
-      <c r="B7" s="33"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="14" t="s">
         <v>38</v>
       </c>
@@ -1767,10 +1770,10 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="18.75">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="35">
         <v>2</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -1785,10 +1788,10 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="18.75">
-      <c r="A9" s="32"/>
-      <c r="B9" s="33"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="11" t="s">
-        <v>37</v>
+        <v>105</v>
       </c>
       <c r="E9" s="23" t="s">
         <v>8</v>
@@ -1801,8 +1804,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A10" s="32"/>
-      <c r="B10" s="33"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="14" t="s">
         <v>38</v>
       </c>
@@ -1815,10 +1818,10 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="18.75">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="33">
+      <c r="B11" s="35">
         <v>3</v>
       </c>
       <c r="C11" s="10" t="s">
@@ -1833,8 +1836,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="18.75">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="11" t="s">
         <v>37</v>
       </c>
@@ -1847,8 +1850,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33"/>
+      <c r="A13" s="31"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="14" t="s">
         <v>38</v>
       </c>
@@ -1861,10 +1864,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="18.75">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="35">
         <v>4</v>
       </c>
       <c r="C14" s="15" t="s">
@@ -1879,8 +1882,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75">
-      <c r="A15" s="34"/>
-      <c r="B15" s="33"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="35"/>
       <c r="C15" s="16" t="s">
         <v>37</v>
       </c>
@@ -1893,8 +1896,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A16" s="34"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="17" t="s">
         <v>38</v>
       </c>
@@ -1907,10 +1910,10 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="18.75">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="33">
+      <c r="B17" s="35">
         <v>5</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -1920,35 +1923,35 @@
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:7" ht="18.75">
-      <c r="A18" s="32"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="11" t="s">
         <v>37</v>
       </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
     </row>
     <row r="19" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A19" s="32"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="36" t="s">
+      <c r="E19" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
     </row>
     <row r="20" spans="1:7" ht="18.75">
-      <c r="A20" s="32" t="s">
+      <c r="A20" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="33">
+      <c r="B20" s="35">
         <v>6</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -1956,40 +1959,40 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="18.75">
-      <c r="A21" s="32"/>
-      <c r="B21" s="33"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="35"/>
       <c r="C21" s="11" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A22" s="32"/>
-      <c r="B22" s="33"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:7" ht="18.75">
-      <c r="A23" s="32"/>
-      <c r="B23" s="33"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="10"/>
     </row>
     <row r="24" spans="1:7" ht="18.75">
-      <c r="A24" s="32"/>
-      <c r="B24" s="33"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="11"/>
     </row>
     <row r="25" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A25" s="32"/>
-      <c r="B25" s="33"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="14"/>
     </row>
     <row r="26" spans="1:7" ht="18.75">
-      <c r="A26" s="32" t="s">
+      <c r="A26" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="31" t="s">
+      <c r="B26" s="32" t="s">
         <v>42</v>
       </c>
       <c r="C26" s="10" t="s">
@@ -1997,38 +2000,38 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="18.75">
-      <c r="A27" s="32"/>
-      <c r="B27" s="31"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="32"/>
       <c r="C27" s="11" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18.75">
-      <c r="A28" s="32"/>
-      <c r="B28" s="31"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="32"/>
       <c r="C28" s="12" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="18.75">
-      <c r="A29" s="32"/>
-      <c r="B29" s="31"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="32"/>
       <c r="C29" s="12" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="19.5" thickBot="1">
-      <c r="A30" s="32"/>
-      <c r="B30" s="31"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="32"/>
       <c r="C30" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="18.75">
-      <c r="A31" s="32" t="s">
+      <c r="A31" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B31" s="32" t="s">
         <v>47</v>
       </c>
       <c r="C31" s="20" t="s">
@@ -2036,44 +2039,44 @@
       </c>
     </row>
     <row r="32" spans="1:7" ht="18.75">
-      <c r="A32" s="32"/>
-      <c r="B32" s="31"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="32"/>
       <c r="C32" s="12" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="18.75">
-      <c r="A33" s="32"/>
-      <c r="B33" s="31"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="32"/>
       <c r="C33" s="16" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A34" s="32"/>
-      <c r="B34" s="31"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="32"/>
       <c r="C34" s="13" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="18.75">
-      <c r="A35" s="32"/>
-      <c r="B35" s="31"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="32"/>
       <c r="C35" s="10"/>
     </row>
     <row r="36" spans="1:13" ht="18.75">
-      <c r="A36" s="32"/>
-      <c r="B36" s="31"/>
+      <c r="A36" s="31"/>
+      <c r="B36" s="32"/>
       <c r="C36" s="11"/>
     </row>
     <row r="37" spans="1:13" ht="18.75">
-      <c r="A37" s="32"/>
-      <c r="B37" s="31"/>
+      <c r="A37" s="31"/>
+      <c r="B37" s="32"/>
       <c r="C37" s="12"/>
     </row>
     <row r="38" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A38" s="32"/>
-      <c r="B38" s="31"/>
+      <c r="A38" s="31"/>
+      <c r="B38" s="32"/>
       <c r="C38" s="13"/>
       <c r="G38" s="29"/>
       <c r="H38" s="29"/>
@@ -2084,10 +2087,10 @@
       <c r="M38" s="29"/>
     </row>
     <row r="39" spans="1:13" ht="18.75">
-      <c r="A39" s="32" t="s">
+      <c r="A39" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="32" t="s">
         <v>52</v>
       </c>
       <c r="C39" s="10" t="s">
@@ -2102,8 +2105,8 @@
       <c r="M39" s="29"/>
     </row>
     <row r="40" spans="1:13" ht="18.75">
-      <c r="A40" s="32"/>
-      <c r="B40" s="31"/>
+      <c r="A40" s="31"/>
+      <c r="B40" s="32"/>
       <c r="C40" s="11" t="s">
         <v>54</v>
       </c>
@@ -2116,8 +2119,8 @@
       <c r="M40" s="29"/>
     </row>
     <row r="41" spans="1:13" ht="18.75">
-      <c r="A41" s="32"/>
-      <c r="B41" s="31"/>
+      <c r="A41" s="31"/>
+      <c r="B41" s="32"/>
       <c r="C41" s="21" t="s">
         <v>55</v>
       </c>
@@ -2130,8 +2133,8 @@
       <c r="M41" s="29"/>
     </row>
     <row r="42" spans="1:13" ht="18.75">
-      <c r="A42" s="32"/>
-      <c r="B42" s="31"/>
+      <c r="A42" s="31"/>
+      <c r="B42" s="32"/>
       <c r="C42" s="11" t="s">
         <v>56</v>
       </c>
@@ -2144,8 +2147,8 @@
       <c r="M42" s="29"/>
     </row>
     <row r="43" spans="1:13" ht="18.75">
-      <c r="A43" s="32"/>
-      <c r="B43" s="31"/>
+      <c r="A43" s="31"/>
+      <c r="B43" s="32"/>
       <c r="C43" s="12" t="s">
         <v>57</v>
       </c>
@@ -2158,8 +2161,8 @@
       <c r="M43" s="29"/>
     </row>
     <row r="44" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A44" s="32"/>
-      <c r="B44" s="31"/>
+      <c r="A44" s="31"/>
+      <c r="B44" s="32"/>
       <c r="C44" s="19" t="s">
         <v>58</v>
       </c>
@@ -2172,10 +2175,10 @@
       <c r="M44" s="29"/>
     </row>
     <row r="45" spans="1:13" ht="18.75">
-      <c r="A45" s="32" t="s">
+      <c r="A45" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="31" t="s">
+      <c r="B45" s="32" t="s">
         <v>60</v>
       </c>
       <c r="C45" s="10" t="s">
@@ -2190,8 +2193,8 @@
       <c r="M45" s="29"/>
     </row>
     <row r="46" spans="1:13" ht="18.75">
-      <c r="A46" s="32"/>
-      <c r="B46" s="31"/>
+      <c r="A46" s="31"/>
+      <c r="B46" s="32"/>
       <c r="C46" s="11" t="s">
         <v>102</v>
       </c>
@@ -2204,8 +2207,8 @@
       <c r="M46" s="29"/>
     </row>
     <row r="47" spans="1:13" ht="18.75">
-      <c r="A47" s="32"/>
-      <c r="B47" s="31"/>
+      <c r="A47" s="31"/>
+      <c r="B47" s="32"/>
       <c r="C47" s="11" t="s">
         <v>103</v>
       </c>
@@ -2218,8 +2221,8 @@
       <c r="M47" s="29"/>
     </row>
     <row r="48" spans="1:13" ht="18.75">
-      <c r="A48" s="32"/>
-      <c r="B48" s="31"/>
+      <c r="A48" s="31"/>
+      <c r="B48" s="32"/>
       <c r="C48" s="11" t="s">
         <v>104</v>
       </c>
@@ -2232,8 +2235,8 @@
       <c r="M48" s="29"/>
     </row>
     <row r="49" spans="1:13" ht="18.75">
-      <c r="A49" s="32"/>
-      <c r="B49" s="31"/>
+      <c r="A49" s="31"/>
+      <c r="B49" s="32"/>
       <c r="C49" s="12" t="s">
         <v>61</v>
       </c>
@@ -2246,8 +2249,8 @@
       <c r="M49" s="29"/>
     </row>
     <row r="50" spans="1:13" ht="18.75">
-      <c r="A50" s="32"/>
-      <c r="B50" s="31"/>
+      <c r="A50" s="31"/>
+      <c r="B50" s="32"/>
       <c r="C50" s="12" t="s">
         <v>62</v>
       </c>
@@ -2260,8 +2263,8 @@
       <c r="M50" s="29"/>
     </row>
     <row r="51" spans="1:13" ht="18.75">
-      <c r="A51" s="32"/>
-      <c r="B51" s="31"/>
+      <c r="A51" s="31"/>
+      <c r="B51" s="32"/>
       <c r="C51" s="11" t="s">
         <v>100</v>
       </c>
@@ -2274,8 +2277,8 @@
       <c r="M51" s="29"/>
     </row>
     <row r="52" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A52" s="32"/>
-      <c r="B52" s="31"/>
+      <c r="A52" s="31"/>
+      <c r="B52" s="32"/>
       <c r="C52" s="14" t="s">
         <v>83</v>
       </c>
@@ -2288,10 +2291,10 @@
       <c r="M52" s="29"/>
     </row>
     <row r="53" spans="1:13" ht="18.75">
-      <c r="A53" s="32" t="s">
+      <c r="A53" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="B53" s="31" t="s">
+      <c r="B53" s="32" t="s">
         <v>63</v>
       </c>
       <c r="C53" s="15" t="s">
@@ -2306,8 +2309,8 @@
       <c r="M53" s="29"/>
     </row>
     <row r="54" spans="1:13" ht="18.75">
-      <c r="A54" s="32"/>
-      <c r="B54" s="31"/>
+      <c r="A54" s="31"/>
+      <c r="B54" s="32"/>
       <c r="C54" s="11" t="s">
         <v>65</v>
       </c>
@@ -2320,8 +2323,8 @@
       <c r="M54" s="29"/>
     </row>
     <row r="55" spans="1:13" ht="18.75">
-      <c r="A55" s="32"/>
-      <c r="B55" s="31"/>
+      <c r="A55" s="31"/>
+      <c r="B55" s="32"/>
       <c r="C55" s="16" t="s">
         <v>66</v>
       </c>
@@ -2334,28 +2337,46 @@
       <c r="M55" s="29"/>
     </row>
     <row r="56" spans="1:13" ht="18.75">
-      <c r="A56" s="32"/>
-      <c r="B56" s="31"/>
+      <c r="A56" s="31"/>
+      <c r="B56" s="32"/>
       <c r="C56" s="11" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="18.75">
-      <c r="A57" s="32"/>
-      <c r="B57" s="31"/>
+      <c r="A57" s="31"/>
+      <c r="B57" s="32"/>
       <c r="C57" s="12" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="19.5" thickBot="1">
-      <c r="A58" s="32"/>
-      <c r="B58" s="31"/>
+      <c r="A58" s="31"/>
+      <c r="B58" s="32"/>
       <c r="C58" s="13" t="s">
         <v>68</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="B39:B44"/>
+    <mergeCell ref="A45:A52"/>
+    <mergeCell ref="B45:B52"/>
+    <mergeCell ref="A53:A58"/>
+    <mergeCell ref="B53:B58"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="B17:B19"/>
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="E19:G19"/>
     <mergeCell ref="A31:A34"/>
@@ -2368,24 +2389,6 @@
     <mergeCell ref="B23:B25"/>
     <mergeCell ref="A26:A30"/>
     <mergeCell ref="B26:B30"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A39:A44"/>
-    <mergeCell ref="B39:B44"/>
-    <mergeCell ref="A45:A52"/>
-    <mergeCell ref="B45:B52"/>
-    <mergeCell ref="A53:A58"/>
-    <mergeCell ref="B53:B58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>

</xml_diff>